<commit_message>
My first_way to Python World! Add work with rows and other functions of type string! Work with dictionary, check attributes in dictionary, Work with cycle for, files, binary numbers and others The end of introduction and the begining of the swim Every thing is ok now Work with numbers(quantitys) Continued The strings continued Strings metods, formating metods The end of Strings and the begining of Lists The end of List and the begining of dictionary To continue working with the dictionary The end working with Dictionary, begins work with Cortege and Files Begins with Operators Learns about operator if, try and cycle while: First program On Python Begins work with operators Python Work with operator "print" End work with if End work with cycles while, for, else End work with chapter 13 and with cycles. It's begin chapter 14 - iteration and includes. To continue iteration and list includes The end of Chapter 3. Begins to do the home task of this chapter.
</commit_message>
<xml_diff>
--- a/149_0503124-3_TOFK_2020_04_07_05_57_17.xlsx
+++ b/149_0503124-3_TOFK_2020_04_07_05_57_17.xlsx
@@ -8993,15 +8993,16 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" customWidth="1"/>
     <col min="7" max="11" width="22.1640625" customWidth="1"/>
   </cols>
@@ -9041,7 +9042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -9076,7 +9077,7 @@
         <v>7613000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -9111,7 +9112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -9146,7 +9147,7 @@
         <v>631147900</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -9181,7 +9182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -9216,7 +9217,7 @@
         <v>493649400</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -9251,7 +9252,7 @@
         <v>253079900</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -9286,7 +9287,7 @@
         <v>31926500</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -9321,7 +9322,7 @@
         <v>10917800</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -9356,7 +9357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -9391,7 +9392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -9426,7 +9427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -9461,7 +9462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -9496,7 +9497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -9531,7 +9532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -9566,7 +9567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -9601,7 +9602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -9636,7 +9637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
@@ -9671,7 +9672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -9706,7 +9707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -9741,7 +9742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -9776,7 +9777,7 @@
         <v>86882700</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -9811,7 +9812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
@@ -9846,7 +9847,7 @@
         <v>69873600</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>11</v>
       </c>
@@ -9881,7 +9882,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>11</v>
       </c>
@@ -9916,7 +9917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>11</v>
       </c>
@@ -9953,5 +9954,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>